<commit_message>
Added plan to make Pecha Kucha presentation
</commit_message>
<xml_diff>
--- a/TimeSheetTemplate.xlsx
+++ b/TimeSheetTemplate.xlsx
@@ -36,7 +36,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="75">
+  <si>
+    <t xml:space="preserve">Monthly timesheet for MSc Geoinformatics IP </t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up Landsat image transfer (~70 images) for possible use case with Martin inc</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project Management class, part II</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work on first draft of Risk Matrix, Gantt and PERT Charts in ProjectLibre</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn Git, create GitHub repository, including excel documents</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create Pecha Kucha Presentation</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
   <si>
     <t>ProjectLibre Tutorials and improving charts</t>
     <phoneticPr fontId="32" type="noConversion"/>
@@ -47,10 +71,6 @@
   </si>
   <si>
     <t>Python Tutorial</t>
-    <phoneticPr fontId="32" type="noConversion"/>
-  </si>
-  <si>
-    <t>Learn Git, create GitHub repository, including excel documents</t>
     <phoneticPr fontId="32" type="noConversion"/>
   </si>
   <si>
@@ -281,32 +301,16 @@
     <t>Meeting with I3 Professors and editing abstract, incl. travel time</t>
     <phoneticPr fontId="32" type="noConversion"/>
   </si>
-  <si>
-    <t xml:space="preserve">Monthly timesheet for MSc Geoinformatics IP </t>
-    <phoneticPr fontId="32" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up Landsat image transfer (~70 images) for possible use case with Martin inc</t>
-    <phoneticPr fontId="32" type="noConversion"/>
-  </si>
-  <si>
-    <t>Project Management class, part II</t>
-    <phoneticPr fontId="32" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work on first draft of Risk Matrix, Gantt and PERT Charts in ProjectLibre</t>
-    <phoneticPr fontId="32" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="198" formatCode="dd/mm/yy;@"/>
-    <numFmt numFmtId="199" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
-    <numFmt numFmtId="208" formatCode="h:mm;@"/>
-    <numFmt numFmtId="216" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -1098,7 +1102,7 @@
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="199" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1121,7 +1125,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="198" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1140,7 +1144,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="198" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1171,42 +1175,93 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="216" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="208" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="216" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="208" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1215,26 +1270,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="216" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="216" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="216" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="216" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1283,56 +1319,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="216" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="216" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="216" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="216" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1808,17 +1812,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="7" customFormat="1" ht="18" thickBot="1">
-      <c r="A1" s="90" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="A1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -1861,15 +1865,15 @@
       <c r="AW1" s="8"/>
     </row>
     <row r="2" spans="1:50" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -1912,16 +1916,16 @@
       <c r="AW2" s="9"/>
     </row>
     <row r="3" spans="1:50" s="11" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="A3" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="23"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -1966,29 +1970,29 @@
       <c r="AX3" s="10"/>
     </row>
     <row r="4" spans="1:50" s="6" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:50" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A5" s="96" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="86"/>
+      <c r="A5" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="23"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -1996,77 +2000,77 @@
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:50" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="87"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
     </row>
     <row r="7" spans="1:50" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A7" s="88" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
+      <c r="A7" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:50" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="1:50" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A9" s="88" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="84" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="86"/>
+      <c r="A9" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
       <c r="I9" s="24"/>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:50" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="95"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
     </row>
     <row r="11" spans="1:50" s="1" customFormat="1" ht="12">
       <c r="A11" s="21" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -2086,55 +2090,55 @@
       <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:50" s="2" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A13" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
+      <c r="A13" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="83"/>
     </row>
     <row r="14" spans="1:50" s="2" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="85"/>
+      <c r="D14" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="90"/>
     </row>
     <row r="15" spans="1:50" ht="13" customHeight="1">
-      <c r="A15" s="70"/>
+      <c r="A15" s="80"/>
       <c r="B15" s="32" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="83"/>
+        <v>21</v>
+      </c>
+      <c r="D15" s="87"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="93"/>
     </row>
     <row r="16" spans="1:50" s="51" customFormat="1" ht="12">
       <c r="A16" s="48" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" s="49">
         <v>0.33333333333333331</v>
@@ -2146,17 +2150,17 @@
         <f>C16-B16</f>
         <v>0.20833333333333331</v>
       </c>
-      <c r="E16" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="59"/>
+      <c r="E16" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="76"/>
     </row>
     <row r="17" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A17" s="48" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B17" s="49"/>
       <c r="C17" s="50"/>
@@ -2164,15 +2168,15 @@
         <f t="shared" ref="D17:D49" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="76"/>
     </row>
     <row r="18" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A18" s="40" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
@@ -2180,15 +2184,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A19" s="40" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B19" s="41">
         <v>0.66666666666666663</v>
@@ -2200,17 +2204,17 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="E19" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="62"/>
+      <c r="E19" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
     </row>
     <row r="20" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A20" s="40" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
@@ -2218,15 +2222,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A21" s="40" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
@@ -2234,15 +2238,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="62"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="59"/>
     </row>
     <row r="22" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A22" s="40" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
@@ -2250,15 +2254,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="60"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="62"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="59"/>
     </row>
     <row r="23" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A23" s="48" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B23" s="49"/>
       <c r="C23" s="50"/>
@@ -2266,15 +2270,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="57"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="59"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="76"/>
     </row>
     <row r="24" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A24" s="48" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B24" s="49">
         <v>0.5</v>
@@ -2286,17 +2290,17 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E24" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="59"/>
+      <c r="E24" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="76"/>
     </row>
     <row r="25" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A25" s="40" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B25" s="41">
         <v>0.625</v>
@@ -2308,17 +2312,17 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E25" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
+      <c r="E25" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A26" s="40" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B26" s="41">
         <v>0.375</v>
@@ -2330,13 +2334,13 @@
         <f>C26-B26</f>
         <v>0.125</v>
       </c>
-      <c r="E26" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62"/>
+      <c r="E26" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A27" s="40"/>
@@ -2350,17 +2354,17 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E27" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62"/>
+      <c r="E27" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A28" s="40" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B28" s="41">
         <v>0.83333333333333337</v>
@@ -2372,17 +2376,17 @@
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="E28" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
+      <c r="E28" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A29" s="40" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B29" s="41">
         <v>0.5</v>
@@ -2394,17 +2398,17 @@
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="E29" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="62"/>
+      <c r="E29" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A30" s="40" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="42"/>
@@ -2412,15 +2416,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="62"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="59"/>
     </row>
     <row r="31" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A31" s="48" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B31" s="49"/>
       <c r="C31" s="50"/>
@@ -2428,15 +2432,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="57"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="59"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="76"/>
     </row>
     <row r="32" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A32" s="48" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B32" s="49"/>
       <c r="C32" s="50"/>
@@ -2444,15 +2448,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="76"/>
     </row>
     <row r="33" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A33" s="40" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
@@ -2460,15 +2464,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="60"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A34" s="40" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
@@ -2476,15 +2480,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="60"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="62"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A35" s="40" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
@@ -2492,15 +2496,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="62"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A36" s="40" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
@@ -2508,15 +2512,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="60"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="62"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A37" s="40" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
@@ -2524,15 +2528,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="62"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="59"/>
     </row>
     <row r="38" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A38" s="48" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B38" s="49"/>
       <c r="C38" s="50"/>
@@ -2540,15 +2544,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="57"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="59"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="76"/>
     </row>
     <row r="39" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A39" s="48" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B39" s="49"/>
       <c r="C39" s="50"/>
@@ -2556,15 +2560,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="57"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="59"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="76"/>
     </row>
     <row r="40" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A40" s="40" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B40" s="41">
         <v>0.9375</v>
@@ -2576,17 +2580,17 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E40" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="62"/>
+      <c r="E40" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="59"/>
     </row>
     <row r="41" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A41" s="40" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B41" s="41">
         <v>0.41666666666666669</v>
@@ -2598,13 +2602,13 @@
         <f t="shared" si="0"/>
         <v>0.12499999999999994</v>
       </c>
-      <c r="E41" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="62"/>
+      <c r="E41" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="59"/>
     </row>
     <row r="42" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A42" s="40"/>
@@ -2618,13 +2622,13 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E42" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="62"/>
+      <c r="E42" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="59"/>
     </row>
     <row r="43" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A43" s="40"/>
@@ -2638,17 +2642,17 @@
         <f t="shared" si="0"/>
         <v>0.10416666666666663</v>
       </c>
-      <c r="E43" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="62"/>
+      <c r="E43" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="59"/>
     </row>
     <row r="44" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A44" s="40" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B44" s="41">
         <v>0.5</v>
@@ -2660,17 +2664,17 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E44" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="62"/>
+      <c r="E44" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="59"/>
     </row>
     <row r="45" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A45" s="40" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B45" s="41">
         <v>0.41666666666666669</v>
@@ -2682,17 +2686,17 @@
         <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="E45" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="62"/>
+      <c r="E45" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="59"/>
     </row>
     <row r="46" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A46" s="40" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B46" s="41">
         <v>0.5</v>
@@ -2704,17 +2708,17 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E46" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="62"/>
+      <c r="E46" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="59"/>
     </row>
     <row r="47" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A47" s="48" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B47" s="49"/>
       <c r="C47" s="50"/>
@@ -2722,15 +2726,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E47" s="57"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="59"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
+      <c r="I47" s="76"/>
     </row>
     <row r="48" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A48" s="48" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B48" s="49"/>
       <c r="C48" s="50"/>
@@ -2738,15 +2742,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E48" s="57"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="59"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="76"/>
     </row>
     <row r="49" spans="1:13" s="43" customFormat="1" ht="12">
       <c r="A49" s="44" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B49" s="41">
         <v>0.5</v>
@@ -2758,27 +2762,27 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E49" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="62"/>
+      <c r="E49" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="59"/>
     </row>
     <row r="50" spans="1:13" s="47" customFormat="1" ht="13">
-      <c r="A50" s="63"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
+      <c r="A50" s="94"/>
+      <c r="B50" s="95"/>
+      <c r="C50" s="95"/>
       <c r="D50" s="46">
         <f>SUM(D16:D49)</f>
         <v>1.65625</v>
       </c>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-      <c r="I50" s="66"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="97"/>
     </row>
     <row r="51" spans="1:13" ht="7.5" customHeight="1">
       <c r="A51" s="28"/>
@@ -2811,6 +2815,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E48:I48"/>
+    <mergeCell ref="E49:I49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="E50:I50"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
@@ -2827,44 +2869,6 @@
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="E18:I18"/>
     <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:I15"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E48:I48"/>
-    <mergeCell ref="E49:I49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="E50:I50"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2886,7 +2890,7 @@
   <dimension ref="A1:AS47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:I36"/>
+      <selection activeCell="E35" sqref="E35:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="10"/>
@@ -2904,17 +2908,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" s="7" customFormat="1" ht="18" thickBot="1">
-      <c r="A1" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="A1" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -2952,15 +2956,15 @@
       <c r="AR1" s="8"/>
     </row>
     <row r="2" spans="1:45" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -2998,16 +3002,16 @@
       <c r="AR2" s="9"/>
     </row>
     <row r="3" spans="1:45" s="11" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="A3" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="23"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -3047,112 +3051,112 @@
       <c r="AS3" s="10"/>
     </row>
     <row r="4" spans="1:45" s="6" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:45" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A5" s="96" t="str">
+      <c r="A5" s="70" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="84" t="str">
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="66" t="str">
         <f>October!D5</f>
         <v>Augustin Hannah</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="86"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="23"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:45" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="87"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
     </row>
     <row r="7" spans="1:45" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A7" s="88" t="str">
+      <c r="A7" s="65" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89" t="str">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="73" t="str">
         <f>October!D7</f>
         <v>AIQ</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="1:45" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A9" s="88" t="str">
+      <c r="A9" s="65" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="84" t="str">
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="66" t="str">
         <f>October!D9</f>
         <v>Automating change detection in ImageQuerying</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="86"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
       <c r="I9" s="24"/>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:45" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="95"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
     </row>
     <row r="11" spans="1:45" s="1" customFormat="1" ht="12">
       <c r="A11" s="21" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -3172,55 +3176,55 @@
       <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:45" s="2" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A13" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
+      <c r="A13" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="83"/>
     </row>
     <row r="14" spans="1:45" s="2" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="85"/>
+      <c r="D14" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="90"/>
     </row>
     <row r="15" spans="1:45" ht="13" customHeight="1">
-      <c r="A15" s="70"/>
+      <c r="A15" s="80"/>
       <c r="B15" s="32" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="83"/>
+        <v>21</v>
+      </c>
+      <c r="D15" s="87"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="93"/>
     </row>
     <row r="16" spans="1:45" s="43" customFormat="1" ht="12">
       <c r="A16" s="40" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
@@ -3228,15 +3232,15 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="62"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A17" s="40" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -3244,15 +3248,15 @@
         <f t="shared" ref="D17:D45" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A18" s="40" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
@@ -3260,15 +3264,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A19" s="40" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B19" s="41">
         <v>0.58333333333333337</v>
@@ -3280,17 +3284,17 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E19" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="62"/>
+      <c r="E19" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
     </row>
     <row r="20" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A20" s="48" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="50"/>
@@ -3298,15 +3302,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="59"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="76"/>
     </row>
     <row r="21" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A21" s="48" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B21" s="49"/>
       <c r="C21" s="50"/>
@@ -3314,15 +3318,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="59"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="76"/>
     </row>
     <row r="22" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A22" s="40" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B22" s="41">
         <v>0.39583333333333331</v>
@@ -3334,17 +3338,17 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666669</v>
       </c>
-      <c r="E22" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="62"/>
+      <c r="E22" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="59"/>
     </row>
     <row r="23" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A23" s="40" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B23" s="41">
         <v>0.41666666666666669</v>
@@ -3356,17 +3360,17 @@
         <f t="shared" si="0"/>
         <v>0.12499999999999994</v>
       </c>
-      <c r="E23" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="62"/>
+      <c r="E23" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="59"/>
     </row>
     <row r="24" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A24" s="40" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
@@ -3374,15 +3378,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="60"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="62"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="59"/>
     </row>
     <row r="25" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A25" s="40" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B25" s="41">
         <v>0.75</v>
@@ -3394,17 +3398,17 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E25" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
+      <c r="E25" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A26" s="40" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="42"/>
@@ -3412,15 +3416,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="60"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A27" s="48" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B27" s="49"/>
       <c r="C27" s="50"/>
@@ -3428,15 +3432,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="59"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="76"/>
     </row>
     <row r="28" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A28" s="48" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B28" s="49">
         <v>0.45833333333333331</v>
@@ -3448,17 +3452,17 @@
         <f t="shared" si="0"/>
         <v>0.25000000000000006</v>
       </c>
-      <c r="E28" s="57" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="59"/>
+      <c r="E28" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="76"/>
     </row>
     <row r="29" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A29" s="40" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B29" s="41">
         <v>0.70833333333333337</v>
@@ -3470,17 +3474,17 @@
         <f t="shared" si="0"/>
         <v>0.20833333333333326</v>
       </c>
-      <c r="E29" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="62"/>
+      <c r="E29" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A30" s="40" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B30" s="41">
         <v>0.66666666666666663</v>
@@ -3492,17 +3496,17 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666674</v>
       </c>
-      <c r="E30" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="62"/>
+      <c r="E30" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="59"/>
     </row>
     <row r="31" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A31" s="40" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
@@ -3510,15 +3514,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="60"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="62"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A32" s="40" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
@@ -3526,15 +3530,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="60"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="62"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
     </row>
     <row r="33" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A33" s="40" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
@@ -3542,15 +3546,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="60"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
+      <c r="E33" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A34" s="48" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B34" s="49"/>
       <c r="C34" s="50"/>
@@ -3558,15 +3564,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="57"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="59"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="76"/>
     </row>
     <row r="35" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A35" s="48" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B35" s="49"/>
       <c r="C35" s="50"/>
@@ -3574,15 +3580,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="57"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="59"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="76"/>
     </row>
     <row r="36" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A36" s="40" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
@@ -3590,15 +3596,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="60"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="62"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A37" s="40" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
@@ -3606,15 +3612,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="62"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="59"/>
     </row>
     <row r="38" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A38" s="40" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
@@ -3622,15 +3628,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="60"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="61"/>
-      <c r="I38" s="62"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="59"/>
     </row>
     <row r="39" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A39" s="40" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
@@ -3638,15 +3644,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="60"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="62"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="59"/>
     </row>
     <row r="40" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A40" s="40" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B40" s="41"/>
       <c r="C40" s="42"/>
@@ -3654,15 +3660,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="60"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="62"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="59"/>
     </row>
     <row r="41" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A41" s="48" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B41" s="49"/>
       <c r="C41" s="50"/>
@@ -3670,15 +3676,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="59"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="76"/>
     </row>
     <row r="42" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A42" s="48" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B42" s="49"/>
       <c r="C42" s="50"/>
@@ -3686,15 +3692,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="57"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="59"/>
+      <c r="E42" s="77"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="76"/>
     </row>
     <row r="43" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A43" s="40" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
@@ -3702,15 +3708,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="60"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="62"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="59"/>
     </row>
     <row r="44" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A44" s="40" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B44" s="41"/>
       <c r="C44" s="42"/>
@@ -3718,15 +3724,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="60"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="62"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="59"/>
     </row>
     <row r="45" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A45" s="40" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
@@ -3734,25 +3740,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E45" s="60"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="62"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="59"/>
     </row>
     <row r="46" spans="1:12" s="47" customFormat="1" ht="13">
-      <c r="A46" s="63"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="64"/>
+      <c r="A46" s="94"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
       <c r="D46" s="46">
         <f>SUM(D16:D45)</f>
         <v>1.25</v>
       </c>
-      <c r="E46" s="65"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="65"/>
-      <c r="I46" s="66"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
+      <c r="H46" s="96"/>
+      <c r="I46" s="97"/>
     </row>
     <row r="47" spans="1:12" ht="7" customHeight="1">
       <c r="A47" s="28"/>
@@ -3770,16 +3776,36 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="E18:I18"/>
     <mergeCell ref="E17:I17"/>
@@ -3790,36 +3816,16 @@
     <mergeCell ref="E16:I16"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:I13"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E19:I19"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3858,17 +3864,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="7" customFormat="1" ht="18" thickBot="1">
-      <c r="A1" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="A1" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -3901,15 +3907,15 @@
       <c r="AM1" s="8"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -3942,16 +3948,16 @@
       <c r="AM2" s="9"/>
     </row>
     <row r="3" spans="1:40" s="11" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="A3" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="23"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -3986,112 +3992,112 @@
       <c r="AN3" s="10"/>
     </row>
     <row r="4" spans="1:40" s="6" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:40" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A5" s="96" t="str">
+      <c r="A5" s="70" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="84" t="str">
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="66" t="str">
         <f>October!D5</f>
         <v>Augustin Hannah</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="86"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="23"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="87"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
     </row>
     <row r="7" spans="1:40" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A7" s="88" t="str">
+      <c r="A7" s="65" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89" t="str">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="73" t="str">
         <f>October!D7</f>
         <v>AIQ</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="1:40" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A9" s="88" t="str">
+      <c r="A9" s="65" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="84" t="str">
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="66" t="str">
         <f>October!D9</f>
         <v>Automating change detection in ImageQuerying</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="86"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
       <c r="I9" s="24"/>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="95"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
     </row>
     <row r="11" spans="1:40" s="1" customFormat="1" ht="12">
       <c r="A11" s="21" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -4111,55 +4117,55 @@
       <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:40" s="2" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A13" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
+      <c r="A13" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="83"/>
     </row>
     <row r="14" spans="1:40" s="2" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="85"/>
+      <c r="D14" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="90"/>
     </row>
     <row r="15" spans="1:40" ht="13" customHeight="1">
-      <c r="A15" s="70"/>
+      <c r="A15" s="80"/>
       <c r="B15" s="32" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="83"/>
+        <v>21</v>
+      </c>
+      <c r="D15" s="87"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="93"/>
     </row>
     <row r="16" spans="1:40" s="43" customFormat="1" ht="12">
       <c r="A16" s="40" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
@@ -4167,15 +4173,15 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="62"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A17" s="40" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -4183,15 +4189,15 @@
         <f t="shared" ref="D17:D46" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A18" s="48" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B18" s="49"/>
       <c r="C18" s="50"/>
@@ -4199,15 +4205,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="76"/>
     </row>
     <row r="19" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A19" s="48" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="50"/>
@@ -4215,15 +4221,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="59"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="76"/>
     </row>
     <row r="20" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A20" s="40" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
@@ -4231,15 +4237,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A21" s="40" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
@@ -4247,15 +4253,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="62"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="59"/>
     </row>
     <row r="22" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A22" s="40" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
@@ -4263,15 +4269,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="60"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="62"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="59"/>
     </row>
     <row r="23" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A23" s="40" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="42"/>
@@ -4279,15 +4285,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="60"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="62"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="59"/>
     </row>
     <row r="24" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A24" s="40" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
@@ -4295,15 +4301,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="60"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="62"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="59"/>
     </row>
     <row r="25" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A25" s="48" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="50"/>
@@ -4311,15 +4317,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="57"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="76"/>
     </row>
     <row r="26" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A26" s="48" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B26" s="49"/>
       <c r="C26" s="50"/>
@@ -4327,15 +4333,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="57"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="59"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="76"/>
     </row>
     <row r="27" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A27" s="40" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="42"/>
@@ -4343,15 +4349,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="60"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A28" s="40" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
@@ -4359,15 +4365,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="60"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A29" s="40" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="42"/>
@@ -4375,15 +4381,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="62"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A30" s="40" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="42"/>
@@ -4391,15 +4397,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="62"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="59"/>
     </row>
     <row r="31" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A31" s="40" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
@@ -4407,15 +4413,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="60"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="62"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A32" s="48" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B32" s="49"/>
       <c r="C32" s="50"/>
@@ -4423,15 +4429,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="76"/>
     </row>
     <row r="33" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A33" s="48" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B33" s="49"/>
       <c r="C33" s="50"/>
@@ -4439,15 +4445,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="59"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="76"/>
     </row>
     <row r="34" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A34" s="40" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
@@ -4455,15 +4461,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="60"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="62"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A35" s="40" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
@@ -4471,15 +4477,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="62"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A36" s="40" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
@@ -4487,15 +4493,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="60"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="62"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A37" s="40" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
@@ -4503,15 +4509,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="62"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="59"/>
     </row>
     <row r="38" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A38" s="40" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
@@ -4519,15 +4525,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="60"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="61"/>
-      <c r="I38" s="62"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="59"/>
     </row>
     <row r="39" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A39" s="48" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B39" s="49"/>
       <c r="C39" s="50"/>
@@ -4535,15 +4541,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="57"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="59"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="76"/>
     </row>
     <row r="40" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A40" s="48" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B40" s="49"/>
       <c r="C40" s="50"/>
@@ -4551,15 +4557,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="57"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="59"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="76"/>
     </row>
     <row r="41" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A41" s="40" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B41" s="41"/>
       <c r="C41" s="42"/>
@@ -4567,15 +4573,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="60"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="62"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="59"/>
     </row>
     <row r="42" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A42" s="40" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B42" s="41"/>
       <c r="C42" s="42"/>
@@ -4583,15 +4589,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="60"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="62"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="59"/>
     </row>
     <row r="43" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A43" s="40" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
@@ -4599,15 +4605,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="60"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="62"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="59"/>
     </row>
     <row r="44" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A44" s="40" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B44" s="41"/>
       <c r="C44" s="42"/>
@@ -4615,15 +4621,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="60"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="62"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="59"/>
     </row>
     <row r="45" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A45" s="40" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
@@ -4631,15 +4637,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E45" s="60"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="62"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="59"/>
     </row>
     <row r="46" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A46" s="48" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B46" s="49"/>
       <c r="C46" s="50"/>
@@ -4647,11 +4653,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="59"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="75"/>
+      <c r="I46" s="76"/>
     </row>
     <row r="47" spans="1:12" s="35" customFormat="1" ht="13">
       <c r="A47" s="100"/>
@@ -4682,46 +4688,7 @@
       <c r="L48" s="13"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="51">
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
     <mergeCell ref="E41:I41"/>
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="E43:I43"/>
@@ -4735,6 +4702,44 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:I15"/>
     <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A6:I6"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -4773,17 +4778,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="7" customFormat="1" ht="18" thickBot="1">
-      <c r="A1" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="A1" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -4816,15 +4821,15 @@
       <c r="AM1" s="8"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -4857,16 +4862,16 @@
       <c r="AM2" s="9"/>
     </row>
     <row r="3" spans="1:40" s="11" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="A3" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="23"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -4901,112 +4906,112 @@
       <c r="AN3" s="10"/>
     </row>
     <row r="4" spans="1:40" s="6" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:40" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A5" s="96" t="str">
+      <c r="A5" s="70" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="84" t="str">
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="66" t="str">
         <f>October!D5</f>
         <v>Augustin Hannah</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="86"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="23"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="87"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
     </row>
     <row r="7" spans="1:40" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A7" s="88" t="str">
+      <c r="A7" s="65" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89" t="str">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="73" t="str">
         <f>October!D7</f>
         <v>AIQ</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="1:40" s="1" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A9" s="88" t="str">
+      <c r="A9" s="65" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="84" t="str">
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="66" t="str">
         <f>October!D9</f>
         <v>Automating change detection in ImageQuerying</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="86"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
       <c r="I9" s="24"/>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:40" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="95"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
     </row>
     <row r="11" spans="1:40" s="1" customFormat="1" ht="12">
       <c r="A11" s="21" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -5026,55 +5031,55 @@
       <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:40" s="2" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A13" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
+      <c r="A13" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="83"/>
     </row>
     <row r="14" spans="1:40" s="2" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="85"/>
+      <c r="D14" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="90"/>
     </row>
     <row r="15" spans="1:40" ht="12" customHeight="1">
-      <c r="A15" s="70"/>
+      <c r="A15" s="80"/>
       <c r="B15" s="32" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="83"/>
+        <v>21</v>
+      </c>
+      <c r="D15" s="87"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="93"/>
     </row>
     <row r="16" spans="1:40" s="51" customFormat="1" ht="12">
       <c r="A16" s="48" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" s="49"/>
       <c r="C16" s="50"/>
@@ -5082,15 +5087,15 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="59"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="76"/>
     </row>
     <row r="17" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A17" s="40" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -5098,15 +5103,15 @@
         <f t="shared" ref="D17:D46" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A18" s="40" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
@@ -5114,15 +5119,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A19" s="40" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="42"/>
@@ -5130,15 +5135,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="62"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
     </row>
     <row r="20" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A20" s="40" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
@@ -5146,15 +5151,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A21" s="40" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
@@ -5162,15 +5167,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="62"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="59"/>
     </row>
     <row r="22" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A22" s="48" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B22" s="49"/>
       <c r="C22" s="50"/>
@@ -5178,15 +5183,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="59"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="76"/>
     </row>
     <row r="23" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A23" s="48" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B23" s="49"/>
       <c r="C23" s="50"/>
@@ -5194,15 +5199,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="57"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="59"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="76"/>
     </row>
     <row r="24" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A24" s="40" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
@@ -5210,15 +5215,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="60"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="62"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="59"/>
     </row>
     <row r="25" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A25" s="40" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
@@ -5226,15 +5231,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="60"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A26" s="40" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="42"/>
@@ -5242,15 +5247,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="60"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A27" s="40" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="42"/>
@@ -5258,15 +5263,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="60"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A28" s="40" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
@@ -5274,15 +5279,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="60"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A29" s="48" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B29" s="49"/>
       <c r="C29" s="50"/>
@@ -5290,15 +5295,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="59"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="76"/>
     </row>
     <row r="30" spans="1:9" s="51" customFormat="1" ht="12">
       <c r="A30" s="48" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B30" s="49"/>
       <c r="C30" s="50"/>
@@ -5306,15 +5311,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="57"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="59"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="76"/>
     </row>
     <row r="31" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A31" s="40" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
@@ -5322,15 +5327,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="60"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="62"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="1:9" s="43" customFormat="1" ht="12">
       <c r="A32" s="40" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
@@ -5338,15 +5343,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="60"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="62"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
     </row>
     <row r="33" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A33" s="40" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
@@ -5354,15 +5359,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="60"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A34" s="40" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
@@ -5370,15 +5375,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="60"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="62"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A35" s="40" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
@@ -5386,15 +5391,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="62"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A36" s="48" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B36" s="49"/>
       <c r="C36" s="50"/>
@@ -5402,15 +5407,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="57"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="59"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="76"/>
     </row>
     <row r="37" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A37" s="48" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B37" s="49"/>
       <c r="C37" s="50"/>
@@ -5418,15 +5423,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="57"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="59"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="76"/>
     </row>
     <row r="38" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A38" s="40" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
@@ -5434,15 +5439,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="60"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="61"/>
-      <c r="I38" s="62"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="59"/>
     </row>
     <row r="39" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A39" s="40" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
@@ -5450,15 +5455,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="60"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="62"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="59"/>
     </row>
     <row r="40" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A40" s="40" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B40" s="41"/>
       <c r="C40" s="42"/>
@@ -5466,15 +5471,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="60"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="62"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="59"/>
     </row>
     <row r="41" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A41" s="40" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B41" s="41"/>
       <c r="C41" s="42"/>
@@ -5482,15 +5487,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="60"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="62"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="59"/>
     </row>
     <row r="42" spans="1:12" s="43" customFormat="1" ht="12">
       <c r="A42" s="40" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B42" s="41"/>
       <c r="C42" s="42"/>
@@ -5498,15 +5503,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="60"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="62"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="59"/>
     </row>
     <row r="43" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A43" s="48" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B43" s="49"/>
       <c r="C43" s="50"/>
@@ -5514,15 +5519,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="57"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="59"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="76"/>
     </row>
     <row r="44" spans="1:12" s="51" customFormat="1" ht="12">
       <c r="A44" s="48" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B44" s="49"/>
       <c r="C44" s="50"/>
@@ -5530,15 +5535,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="57"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="59"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="75"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="76"/>
     </row>
     <row r="45" spans="1:12" s="39" customFormat="1" ht="12">
       <c r="A45" s="36" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B45" s="37"/>
       <c r="C45" s="38"/>
@@ -5554,7 +5559,7 @@
     </row>
     <row r="46" spans="1:12" s="39" customFormat="1" ht="12">
       <c r="A46" s="36" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B46" s="37"/>
       <c r="C46" s="38"/>
@@ -5597,46 +5602,7 @@
       <c r="L48" s="13"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="51">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
     <mergeCell ref="E36:I36"/>
     <mergeCell ref="E37:I37"/>
     <mergeCell ref="E38:I38"/>
@@ -5650,6 +5616,44 @@
     <mergeCell ref="E44:I44"/>
     <mergeCell ref="E46:I46"/>
     <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>